<commit_message>
shorten up the import controller
</commit_message>
<xml_diff>
--- a/excel_templates/leaseagrm-template.xlsx
+++ b/excel_templates/leaseagrm-template.xlsx
@@ -24,9 +24,6 @@
     <t>Apartment</t>
   </si>
   <si>
-    <t>Tenant_ID</t>
-  </si>
-  <si>
     <t>Start date</t>
   </si>
   <si>
@@ -55,6 +52,9 @@
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Tenant Passport ID Number</t>
   </si>
 </sst>
 </file>
@@ -434,7 +434,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -445,40 +445,40 @@
   <sheetData>
     <row r="1" spans="1:12" ht="39">
       <c r="A1" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>9</v>
-      </c>
-      <c r="L1" s="8" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="15.75">

</xml_diff>

<commit_message>
hot fix - and some of the excel and scrolling done
Former-commit-id: c17fe90ea5aee2caca6c7ff3bbc6340fae769337
</commit_message>
<xml_diff>
--- a/excel_templates/leaseagrm-template.xlsx
+++ b/excel_templates/leaseagrm-template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Apartment</t>
   </si>
@@ -52,20 +52,16 @@
   </si>
   <si>
     <t>Name</t>
-  </si>
-  <si>
-    <t>Tenant Passport ID Number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+  <numFmts count="1">
     <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,15 +79,6 @@
       <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="VNI-Times"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="VNI-Times"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,21 +116,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -431,237 +410,221 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.7109375" customWidth="1"/>
-    <col min="2" max="12" width="13.7109375" customWidth="1"/>
+    <col min="2" max="11" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="39">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:11" ht="39" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="8" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="15.75">
+    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" ht="15.75">
+    </row>
+    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" ht="15.75">
+    </row>
+    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" ht="15.75">
+    </row>
+    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
       <c r="G5" s="3"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" ht="15.75">
+    </row>
+    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
       <c r="G6" s="3"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" ht="15.75">
+    </row>
+    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="1:12" ht="15.75">
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
       <c r="G8" s="3"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-    </row>
-    <row r="9" spans="1:12" ht="15.75">
+    </row>
+    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
       <c r="G9" s="3"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" ht="15.75">
+    </row>
+    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
       <c r="G10" s="3"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-    </row>
-    <row r="11" spans="1:12" ht="15.75">
+    </row>
+    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
       <c r="G11" s="3"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-    </row>
-    <row r="12" spans="1:12" ht="15.75">
+    </row>
+    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
       <c r="G12" s="3"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-    </row>
-    <row r="13" spans="1:12" ht="15.75">
+    </row>
+    <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
       <c r="G13" s="3"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-    </row>
-    <row r="14" spans="1:12" ht="15.75">
+    </row>
+    <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
do couple change when unable to search through and change the overview
</commit_message>
<xml_diff>
--- a/excel_templates/leaseagrm-template.xlsx
+++ b/excel_templates/leaseagrm-template.xlsx
@@ -51,15 +51,16 @@
     <t>Deposit exchange rate</t>
   </si>
   <si>
-    <t>Name</t>
+    <t>Agreement Number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -116,7 +117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -124,11 +125,14 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -413,7 +417,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="C2" sqref="C2:D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,8 +464,8 @@
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="3"/>
@@ -473,8 +477,8 @@
     <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="3"/>
@@ -486,8 +490,8 @@
     <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="3"/>
@@ -499,8 +503,8 @@
     <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
       <c r="G5" s="3"/>
@@ -512,8 +516,8 @@
     <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="3"/>
@@ -525,8 +529,8 @@
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="3"/>
@@ -538,8 +542,8 @@
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="3"/>
@@ -551,8 +555,8 @@
     <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="3"/>
@@ -564,8 +568,8 @@
     <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="3"/>
@@ -577,8 +581,8 @@
     <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="3"/>
@@ -590,8 +594,8 @@
     <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="3"/>
@@ -603,8 +607,8 @@
     <row r="13" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="3"/>
@@ -616,8 +620,8 @@
     <row r="14" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="3"/>

</xml_diff>

<commit_message>
change apartment table to unit
Former-commit-id: ed4ab38643f492bf061c005cda45aeab26f0c0e3
</commit_message>
<xml_diff>
--- a/excel_templates/leaseagrm-template.xlsx
+++ b/excel_templates/leaseagrm-template.xlsx
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
-    <t>Apartment</t>
-  </si>
-  <si>
     <t>Start date</t>
   </si>
   <si>
@@ -64,6 +61,9 @@
   </si>
   <si>
     <t>Tenant ID</t>
+  </si>
+  <si>
+    <t>Unit</t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,48 +478,48 @@
   <sheetData>
     <row r="1" spans="1:13" ht="39" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="13" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>12</v>
       </c>
       <c r="C2" s="11">
         <v>35</v>
@@ -546,13 +546,13 @@
         <v>1</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L2" s="14">
         <v>1</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="9" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>